<commit_message>
Edited error in recommendations
</commit_message>
<xml_diff>
--- a/BL_Input/AnalystRecommendation.xlsx
+++ b/BL_Input/AnalystRecommendation.xlsx
@@ -5,42 +5,41 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miros\Desktop\masters\BL Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miros\Desktop\masters\BL_Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CFEBC4-7A87-47C7-BBD0-EA397E24577D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6694BD1-9419-47A4-909A-C806B3272236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Bond durace" sheetId="2" r:id="rId2"/>
-    <sheet name="SO" sheetId="15" r:id="rId3"/>
-    <sheet name="ABT" sheetId="19" r:id="rId4"/>
-    <sheet name="MNST" sheetId="27" r:id="rId5"/>
-    <sheet name="MOH" sheetId="28" r:id="rId6"/>
-    <sheet name="AIG" sheetId="20" r:id="rId7"/>
-    <sheet name="AKAM" sheetId="21" r:id="rId8"/>
-    <sheet name="DECK" sheetId="25" r:id="rId9"/>
-    <sheet name="DLTR" sheetId="26" r:id="rId10"/>
-    <sheet name="CAG" sheetId="23" r:id="rId11"/>
-    <sheet name="CTRA" sheetId="24" r:id="rId12"/>
-    <sheet name="AXON" sheetId="22" r:id="rId13"/>
-    <sheet name="DVA" sheetId="17" r:id="rId14"/>
-    <sheet name="WEC" sheetId="18" r:id="rId15"/>
-    <sheet name="CNC" sheetId="16" r:id="rId16"/>
-    <sheet name="AEE" sheetId="3" r:id="rId17"/>
-    <sheet name="AEP" sheetId="4" r:id="rId18"/>
-    <sheet name="CMS" sheetId="5" r:id="rId19"/>
-    <sheet name="D" sheetId="6" r:id="rId20"/>
-    <sheet name="DTE" sheetId="7" r:id="rId21"/>
-    <sheet name="DUK" sheetId="8" r:id="rId22"/>
-    <sheet name="ED" sheetId="9" r:id="rId23"/>
-    <sheet name="ES" sheetId="10" r:id="rId24"/>
-    <sheet name="EVRG" sheetId="11" r:id="rId25"/>
-    <sheet name="LNT" sheetId="12" r:id="rId26"/>
-    <sheet name="PNW" sheetId="13" r:id="rId27"/>
-    <sheet name="TKO" sheetId="14" r:id="rId28"/>
+    <sheet name="SO" sheetId="15" r:id="rId2"/>
+    <sheet name="ABT" sheetId="19" r:id="rId3"/>
+    <sheet name="MNST" sheetId="27" r:id="rId4"/>
+    <sheet name="MOH" sheetId="28" r:id="rId5"/>
+    <sheet name="AIG" sheetId="20" r:id="rId6"/>
+    <sheet name="AKAM" sheetId="21" r:id="rId7"/>
+    <sheet name="DECK" sheetId="25" r:id="rId8"/>
+    <sheet name="DLTR" sheetId="26" r:id="rId9"/>
+    <sheet name="CAG" sheetId="23" r:id="rId10"/>
+    <sheet name="CTRA" sheetId="24" r:id="rId11"/>
+    <sheet name="AXON" sheetId="22" r:id="rId12"/>
+    <sheet name="DVA" sheetId="17" r:id="rId13"/>
+    <sheet name="WEC" sheetId="18" r:id="rId14"/>
+    <sheet name="CNC" sheetId="16" r:id="rId15"/>
+    <sheet name="AEE" sheetId="3" r:id="rId16"/>
+    <sheet name="AEP" sheetId="4" r:id="rId17"/>
+    <sheet name="CMS" sheetId="5" r:id="rId18"/>
+    <sheet name="D" sheetId="6" r:id="rId19"/>
+    <sheet name="DTE" sheetId="7" r:id="rId20"/>
+    <sheet name="DUK" sheetId="8" r:id="rId21"/>
+    <sheet name="ED" sheetId="9" r:id="rId22"/>
+    <sheet name="ES" sheetId="10" r:id="rId23"/>
+    <sheet name="EVRG" sheetId="11" r:id="rId24"/>
+    <sheet name="LNT" sheetId="12" r:id="rId25"/>
+    <sheet name="PNW" sheetId="13" r:id="rId26"/>
+    <sheet name="TKO" sheetId="14" r:id="rId27"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="36">
   <si>
     <t>highCorrelationPortfolio</t>
   </si>
@@ -149,42 +148,6 @@
     <t>MOH</t>
   </si>
   <si>
-    <t>CZ0001004477</t>
-  </si>
-  <si>
-    <t>Cena</t>
-  </si>
-  <si>
-    <t>FV</t>
-  </si>
-  <si>
-    <t>Kupon</t>
-  </si>
-  <si>
-    <t>YTM</t>
-  </si>
-  <si>
-    <t>Aktuální datum</t>
-  </si>
-  <si>
-    <t>Datum splatnosti</t>
-  </si>
-  <si>
-    <t>Mdur</t>
-  </si>
-  <si>
-    <t>Dur</t>
-  </si>
-  <si>
-    <t>DV01</t>
-  </si>
-  <si>
-    <t>Pozice</t>
-  </si>
-  <si>
-    <t>Ztráta při růstu o 1bps</t>
-  </si>
-  <si>
     <t>Dates</t>
   </si>
   <si>
@@ -205,41 +168,12 @@
   <si>
     <t>Price Spread</t>
   </si>
-  <si>
-    <t>Horizon</t>
-  </si>
-  <si>
-    <t>Horizon Yield</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Datum emise</t>
-  </si>
-  <si>
-    <t>První úrok (roční)</t>
-  </si>
-  <si>
-    <t>Principal</t>
-  </si>
-  <si>
-    <t>Amnt</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;Kč&quot;_-;\-* #,##0.00\ &quot;Kč&quot;_-;_-* &quot;-&quot;??\ &quot;Kč&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.000%"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;Kč&quot;_-;\-* #,##0\ &quot;Kč&quot;_-;_-* &quot;-&quot;??\ &quot;Kč&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;Kč&quot;"/>
-    <numFmt numFmtId="167" formatCode="#,##0\ &quot;Kč&quot;"/>
-    <numFmt numFmtId="168" formatCode="#,##0.000\ &quot;Kč&quot;"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,13 +187,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -294,33 +221,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Měna" xfId="1" builtinId="4"/>
+  <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
-    <cellStyle name="Procenta" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -623,7 +535,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -761,622 +673,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:G26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B2">
-        <v>159.5</v>
-      </c>
-      <c r="C2">
-        <v>152.36000000000001</v>
-      </c>
-      <c r="D2">
-        <v>0.48275862068965519</v>
-      </c>
-      <c r="E2">
-        <v>0.41379310344827586</v>
-      </c>
-      <c r="F2">
-        <v>0.10344827586206896</v>
-      </c>
-      <c r="G2">
-        <v>7.1399999999999864</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>45071</v>
-      </c>
-      <c r="B3">
-        <v>152.75</v>
-      </c>
-      <c r="C3">
-        <v>136.66</v>
-      </c>
-      <c r="D3">
-        <v>0.48275862068965519</v>
-      </c>
-      <c r="E3">
-        <v>0.41379310344827586</v>
-      </c>
-      <c r="F3">
-        <v>0.10344827586206896</v>
-      </c>
-      <c r="G3">
-        <v>16.090000000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>45102</v>
-      </c>
-      <c r="B4">
-        <v>153</v>
-      </c>
-      <c r="C4">
-        <v>143.66999999999999</v>
-      </c>
-      <c r="D4">
-        <v>0.5</v>
-      </c>
-      <c r="E4">
-        <v>0.39285714285714285</v>
-      </c>
-      <c r="F4">
-        <v>0.10714285714285714</v>
-      </c>
-      <c r="G4">
-        <v>9.3300000000000125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>45132</v>
-      </c>
-      <c r="B5">
-        <v>153.23809814453125</v>
-      </c>
-      <c r="C5">
-        <v>151.91999999999999</v>
-      </c>
-      <c r="D5">
-        <v>0.5</v>
-      </c>
-      <c r="E5">
-        <v>0.39285714285714285</v>
-      </c>
-      <c r="F5">
-        <v>0.10714285714285714</v>
-      </c>
-      <c r="G5">
-        <v>1.3180981445312625</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>45163</v>
-      </c>
-      <c r="B6">
-        <v>149.39131164550781</v>
-      </c>
-      <c r="C6">
-        <v>123.31</v>
-      </c>
-      <c r="D6">
-        <v>0.48275862068965519</v>
-      </c>
-      <c r="E6">
-        <v>0.41379310344827586</v>
-      </c>
-      <c r="F6">
-        <v>0.10344827586206896</v>
-      </c>
-      <c r="G6">
-        <v>26.08131164550781</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>45194</v>
-      </c>
-      <c r="B7">
-        <v>150.5238037109375</v>
-      </c>
-      <c r="C7">
-        <v>104.4</v>
-      </c>
-      <c r="D7">
-        <v>0.51724137931034486</v>
-      </c>
-      <c r="E7">
-        <v>0.37931034482758619</v>
-      </c>
-      <c r="F7">
-        <v>0.10344827586206896</v>
-      </c>
-      <c r="G7">
-        <v>46.123803710937494</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>45224</v>
-      </c>
-      <c r="B8">
-        <v>144.77272033691406</v>
-      </c>
-      <c r="C8">
-        <v>108.3</v>
-      </c>
-      <c r="D8">
-        <v>0.56666666666666665</v>
-      </c>
-      <c r="E8">
-        <v>0.36666666666666664</v>
-      </c>
-      <c r="F8">
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="G8">
-        <v>36.472720336914065</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>45255</v>
-      </c>
-      <c r="B9">
-        <v>142.6842041015625</v>
-      </c>
-      <c r="C9">
-        <v>117.32</v>
-      </c>
-      <c r="D9">
-        <v>0.56666666666666665</v>
-      </c>
-      <c r="E9">
-        <v>0.36666666666666664</v>
-      </c>
-      <c r="F9">
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="G9">
-        <v>25.364204101562507</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>45285</v>
-      </c>
-      <c r="B10">
-        <v>143.52174377441406</v>
-      </c>
-      <c r="C10">
-        <v>136.56</v>
-      </c>
-      <c r="D10">
-        <v>0.56666666666666665</v>
-      </c>
-      <c r="E10">
-        <v>0.36666666666666664</v>
-      </c>
-      <c r="F10">
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="G10">
-        <v>6.9617437744140602</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>45316</v>
-      </c>
-      <c r="B11">
-        <v>145.2608642578125</v>
-      </c>
-      <c r="C11">
-        <v>132.22999999999999</v>
-      </c>
-      <c r="D11">
-        <v>0.56666666666666665</v>
-      </c>
-      <c r="E11">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F11">
-        <v>0.1</v>
-      </c>
-      <c r="G11">
-        <v>13.03086425781251</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>45347</v>
-      </c>
-      <c r="B12">
-        <v>148</v>
-      </c>
-      <c r="C12">
-        <v>145.88</v>
-      </c>
-      <c r="D12">
-        <v>0.6</v>
-      </c>
-      <c r="E12">
-        <v>0.3</v>
-      </c>
-      <c r="F12">
-        <v>0.1</v>
-      </c>
-      <c r="G12">
-        <v>2.1200000000000045</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>45376</v>
-      </c>
-      <c r="B13">
-        <v>148.69564819335938</v>
-      </c>
-      <c r="C13">
-        <v>126.15</v>
-      </c>
-      <c r="D13">
-        <v>0.58620689655172409</v>
-      </c>
-      <c r="E13">
-        <v>0.34482758620689657</v>
-      </c>
-      <c r="F13">
-        <v>6.8965517241379309E-2</v>
-      </c>
-      <c r="G13">
-        <v>22.545648193359369</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>45407</v>
-      </c>
-      <c r="B14">
-        <v>148.65217590332031</v>
-      </c>
-      <c r="C14">
-        <v>121.69</v>
-      </c>
-      <c r="D14">
-        <v>0.55172413793103448</v>
-      </c>
-      <c r="E14">
-        <v>0.37931034482758619</v>
-      </c>
-      <c r="F14">
-        <v>6.8965517241379309E-2</v>
-      </c>
-      <c r="G14">
-        <v>26.962175903320315</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>45437</v>
-      </c>
-      <c r="B15">
-        <v>147.75</v>
-      </c>
-      <c r="C15">
-        <v>115.37</v>
-      </c>
-      <c r="D15">
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="E15">
-        <v>0.35714285714285715</v>
-      </c>
-      <c r="F15">
-        <v>7.1428571428571425E-2</v>
-      </c>
-      <c r="G15">
-        <v>32.379999999999995</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>45468</v>
-      </c>
-      <c r="B16">
-        <v>137.29167175292969</v>
-      </c>
-      <c r="C16">
-        <v>105.41</v>
-      </c>
-      <c r="D16">
-        <v>0.5357142857142857</v>
-      </c>
-      <c r="E16">
-        <v>0.39285714285714285</v>
-      </c>
-      <c r="F16">
-        <v>7.1428571428571425E-2</v>
-      </c>
-      <c r="G16">
-        <v>31.881671752929691</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>45498</v>
-      </c>
-      <c r="B17">
-        <v>136.36000061035156</v>
-      </c>
-      <c r="C17">
-        <v>102.63</v>
-      </c>
-      <c r="D17">
-        <v>0.5</v>
-      </c>
-      <c r="E17">
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="F17">
-        <v>7.1428571428571425E-2</v>
-      </c>
-      <c r="G17">
-        <v>33.730000610351567</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>45529</v>
-      </c>
-      <c r="B18">
-        <v>133</v>
-      </c>
-      <c r="C18">
-        <v>97</v>
-      </c>
-      <c r="D18">
-        <v>0.5357142857142857</v>
-      </c>
-      <c r="E18">
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="F18">
-        <v>3.5714285714285712E-2</v>
-      </c>
-      <c r="G18">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>45560</v>
-      </c>
-      <c r="B19">
-        <v>82.615386962890625</v>
-      </c>
-      <c r="C19">
-        <v>70.55</v>
-      </c>
-      <c r="D19">
-        <v>0.43333333333333335</v>
-      </c>
-      <c r="E19">
-        <v>0.53333333333333333</v>
-      </c>
-      <c r="F19">
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="G19">
-        <v>12.065386962890628</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>45590</v>
-      </c>
-      <c r="B20">
-        <v>83.296295166015625</v>
-      </c>
-      <c r="C20">
-        <v>66.45</v>
-      </c>
-      <c r="D20">
-        <v>0.43333333333333335</v>
-      </c>
-      <c r="E20">
-        <v>0.53333333333333333</v>
-      </c>
-      <c r="F20">
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="G20">
-        <v>16.846295166015622</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>45621</v>
-      </c>
-      <c r="B21">
-        <v>81.615386962890625</v>
-      </c>
-      <c r="C21">
-        <v>69.78</v>
-      </c>
-      <c r="D21">
-        <v>0.36666666666666664</v>
-      </c>
-      <c r="E21">
-        <v>0.6</v>
-      </c>
-      <c r="F21">
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="G21">
-        <v>11.835386962890624</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>45651</v>
-      </c>
-      <c r="B22">
-        <v>83.538459777832031</v>
-      </c>
-      <c r="C22">
-        <v>73.38</v>
-      </c>
-      <c r="D22">
-        <v>0.36666666666666664</v>
-      </c>
-      <c r="E22">
-        <v>0.6</v>
-      </c>
-      <c r="F22">
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="G22">
-        <v>10.158459777832036</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>45682</v>
-      </c>
-      <c r="B23">
-        <v>84.038459777832031</v>
-      </c>
-      <c r="C23">
-        <v>72.48</v>
-      </c>
-      <c r="D23">
-        <v>0.36666666666666664</v>
-      </c>
-      <c r="E23">
-        <v>0.6</v>
-      </c>
-      <c r="F23">
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="G23">
-        <v>11.558459777832027</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>45713</v>
-      </c>
-      <c r="B24">
-        <v>83.653846740722656</v>
-      </c>
-      <c r="C24">
-        <v>76.22</v>
-      </c>
-      <c r="D24">
-        <v>0.36666666666666664</v>
-      </c>
-      <c r="E24">
-        <v>0.6</v>
-      </c>
-      <c r="F24">
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="G24">
-        <v>7.4338467407226574</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>45741</v>
-      </c>
-      <c r="B25">
-        <v>79.941177368164063</v>
-      </c>
-      <c r="C25">
-        <v>67.14</v>
-      </c>
-      <c r="D25">
-        <v>0.36666666666666664</v>
-      </c>
-      <c r="E25">
-        <v>0.6</v>
-      </c>
-      <c r="F25">
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="G25">
-        <v>12.801177368164062</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>45772</v>
-      </c>
-      <c r="B26">
-        <v>82.954544067382813</v>
-      </c>
-      <c r="C26">
-        <v>81.23</v>
-      </c>
-      <c r="D26">
-        <v>0.41379310344827586</v>
-      </c>
-      <c r="E26">
-        <v>0.55172413793103448</v>
-      </c>
-      <c r="F26">
-        <v>3.4482758620689655E-2</v>
-      </c>
-      <c r="G26">
-        <v>1.7245440673828085</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -1391,25 +687,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1992,7 +1288,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -2007,25 +1303,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2608,7 +1904,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -2623,25 +1919,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -3224,7 +2520,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -3239,25 +2535,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -3840,7 +3136,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -3855,25 +3151,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -4456,7 +3752,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -4471,25 +3767,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -5072,7 +4368,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -5090,25 +4386,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -5691,7 +4987,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -5706,25 +5002,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -6307,7 +5603,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -6322,25 +5618,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -6923,262 +6219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="2">
-        <v>42139</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="2">
-        <v>46022</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="2">
-        <v>42505</v>
-      </c>
-      <c r="G3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="6">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="2">
-        <v>45776</v>
-      </c>
-      <c r="G4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="11">
-        <f>H3*(B6/100)</f>
-        <v>8788200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="2">
-        <v>47618</v>
-      </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6">
-        <v>87.882000000000005</v>
-      </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="10"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7">
-        <v>100</v>
-      </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="3">
-        <v>9.4999999999999998E-3</v>
-      </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="5">
-        <f>YIELD(B4,B5,B8,B6,B7,1)</f>
-        <v>3.6212991603235913E-2</v>
-      </c>
-      <c r="H9" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G10">
-        <v>30</v>
-      </c>
-      <c r="H10" s="5">
-        <f>$H$13+(G10/10000)</f>
-        <v>3.9212991603235915E-2</v>
-      </c>
-      <c r="I10">
-        <f t="shared" ref="I10:I16" si="0">PRICE($H$2,$B$5,$B$8,H10,100,1)</f>
-        <v>88.266664975036093</v>
-      </c>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11">
-        <f>DURATION(B4,B5,B8,B9,1)</f>
-        <v>4.8914800916592203</v>
-      </c>
-      <c r="G11">
-        <v>20</v>
-      </c>
-      <c r="H11" s="5">
-        <f>$H$13+(G11/10000)</f>
-        <v>3.8212991603235914E-2</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>88.632795848889231</v>
-      </c>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="4">
-        <f>MDURATION(B4,B5,B8,B9,1)/100</f>
-        <v>4.720535383455373E-2</v>
-      </c>
-      <c r="G12">
-        <v>10</v>
-      </c>
-      <c r="H12" s="5">
-        <f>$H$13+(G12/10000)</f>
-        <v>3.7212991603235913E-2</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>89.000814960318905</v>
-      </c>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13">
-        <f>(B6*B12)/10000</f>
-        <v>4.1485009056882509E-4</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" s="8">
-        <f>B9</f>
-        <v>3.6212991603235913E-2</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>89.370733906772642</v>
-      </c>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G14">
-        <v>-10</v>
-      </c>
-      <c r="H14" s="5">
-        <f>$H$13+(G14/10000)</f>
-        <v>3.5212991603235912E-2</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>89.742564368282729</v>
-      </c>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="6">
-        <v>1000000</v>
-      </c>
-      <c r="G15">
-        <v>-20</v>
-      </c>
-      <c r="H15" s="5">
-        <f t="shared" ref="H15:H16" si="1">$H$13+(G15/10000)</f>
-        <v>3.4212991603235911E-2</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="0"/>
-        <v>90.11631810813563</v>
-      </c>
-      <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="7">
-        <f>B15*B13</f>
-        <v>414.85009056882507</v>
-      </c>
-      <c r="G16">
-        <v>-30</v>
-      </c>
-      <c r="H16" s="5">
-        <f t="shared" si="1"/>
-        <v>3.321299160323591E-2</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="0"/>
-        <v>90.492006973546268</v>
-      </c>
-      <c r="K16" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -7193,25 +6234,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -7794,7 +6835,623 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>45041</v>
+      </c>
+      <c r="B2">
+        <v>72.1875</v>
+      </c>
+      <c r="C2">
+        <v>73.98</v>
+      </c>
+      <c r="D2">
+        <v>0.4</v>
+      </c>
+      <c r="E2">
+        <v>0.4</v>
+      </c>
+      <c r="F2">
+        <v>0.2</v>
+      </c>
+      <c r="G2">
+        <v>-1.792500000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>45071</v>
+      </c>
+      <c r="B3">
+        <v>72.875</v>
+      </c>
+      <c r="C3">
+        <v>69.819999999999993</v>
+      </c>
+      <c r="D3">
+        <v>0.42105263157894735</v>
+      </c>
+      <c r="E3">
+        <v>0.36842105263157893</v>
+      </c>
+      <c r="F3">
+        <v>0.21052631578947367</v>
+      </c>
+      <c r="G3">
+        <v>3.0550000000000068</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>45102</v>
+      </c>
+      <c r="B4">
+        <v>72.800003051757813</v>
+      </c>
+      <c r="C4">
+        <v>70.45</v>
+      </c>
+      <c r="D4">
+        <v>0.45</v>
+      </c>
+      <c r="E4">
+        <v>0.35</v>
+      </c>
+      <c r="F4">
+        <v>0.2</v>
+      </c>
+      <c r="G4">
+        <v>2.3500030517578097</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45132</v>
+      </c>
+      <c r="B5">
+        <v>73.266670227050781</v>
+      </c>
+      <c r="C5">
+        <v>72.61</v>
+      </c>
+      <c r="D5">
+        <v>0.42105263157894735</v>
+      </c>
+      <c r="E5">
+        <v>0.31578947368421051</v>
+      </c>
+      <c r="F5">
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="G5">
+        <v>0.65667022705078182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45163</v>
+      </c>
+      <c r="B6">
+        <v>72.894737243652344</v>
+      </c>
+      <c r="C6">
+        <v>68.09</v>
+      </c>
+      <c r="D6">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="E6">
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="F6">
+        <v>9.5238095238095233E-2</v>
+      </c>
+      <c r="G6">
+        <v>4.8047372436523403</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>45194</v>
+      </c>
+      <c r="B7">
+        <v>73.052635192871094</v>
+      </c>
+      <c r="C7">
+        <v>69.290000000000006</v>
+      </c>
+      <c r="D7">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="E7">
+        <v>0.52380952380952384</v>
+      </c>
+      <c r="F7">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="G7">
+        <v>3.7626351928710875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>45224</v>
+      </c>
+      <c r="B8">
+        <v>72.263160705566406</v>
+      </c>
+      <c r="C8">
+        <v>66.61</v>
+      </c>
+      <c r="D8">
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="E8">
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="F8">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="G8">
+        <v>5.6531607055664068</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>45255</v>
+      </c>
+      <c r="B9">
+        <v>72.263160705566406</v>
+      </c>
+      <c r="C9">
+        <v>69.61</v>
+      </c>
+      <c r="D9">
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="E9">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="F9">
+        <v>9.5238095238095233E-2</v>
+      </c>
+      <c r="G9">
+        <v>2.6531607055664068</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>45285</v>
+      </c>
+      <c r="B10">
+        <v>73.421051025390625</v>
+      </c>
+      <c r="C10">
+        <v>69.44</v>
+      </c>
+      <c r="D10">
+        <v>0.5</v>
+      </c>
+      <c r="E10">
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="F10">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="G10">
+        <v>3.9810510253906273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>45316</v>
+      </c>
+      <c r="B11">
+        <v>74.599998474121094</v>
+      </c>
+      <c r="C11">
+        <v>69.239999999999995</v>
+      </c>
+      <c r="D11">
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="E11">
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="F11">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="G11">
+        <v>5.3599984741210989</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>45347</v>
+      </c>
+      <c r="B12">
+        <v>73.421051025390625</v>
+      </c>
+      <c r="C12">
+        <v>67.69</v>
+      </c>
+      <c r="D12">
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="E12">
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="F12">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="G12">
+        <v>5.7310510253906273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>45376</v>
+      </c>
+      <c r="B13">
+        <v>73.368423461914063</v>
+      </c>
+      <c r="C13">
+        <v>69.760000000000005</v>
+      </c>
+      <c r="D13">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="E13">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F13">
+        <v>9.5238095238095233E-2</v>
+      </c>
+      <c r="G13">
+        <v>3.6084234619140574</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>45407</v>
+      </c>
+      <c r="B14">
+        <v>73.611114501953125</v>
+      </c>
+      <c r="C14">
+        <v>74.37</v>
+      </c>
+      <c r="D14">
+        <v>0.52380952380952384</v>
+      </c>
+      <c r="E14">
+        <v>0.38095238095238093</v>
+      </c>
+      <c r="F14">
+        <v>9.5238095238095233E-2</v>
+      </c>
+      <c r="G14">
+        <v>-0.75888549804687955</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>45437</v>
+      </c>
+      <c r="B15">
+        <v>77.117645263671875</v>
+      </c>
+      <c r="C15">
+        <v>77.75</v>
+      </c>
+      <c r="D15">
+        <v>0.52380952380952384</v>
+      </c>
+      <c r="E15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F15">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="G15">
+        <v>-0.632354736328125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>45468</v>
+      </c>
+      <c r="B16">
+        <v>77.5</v>
+      </c>
+      <c r="C16">
+        <v>78.02</v>
+      </c>
+      <c r="D16">
+        <v>0.52380952380952384</v>
+      </c>
+      <c r="E16">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F16">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="G16">
+        <v>-0.51999999999999602</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>45498</v>
+      </c>
+      <c r="B17">
+        <v>79.184211730957031</v>
+      </c>
+      <c r="C17">
+        <v>81.66</v>
+      </c>
+      <c r="D17">
+        <v>0.52380952380952384</v>
+      </c>
+      <c r="E17">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F17">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="G17">
+        <v>-2.4757882690429653</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>45529</v>
+      </c>
+      <c r="B18">
+        <v>85.65789794921875</v>
+      </c>
+      <c r="C18">
+        <v>86.12</v>
+      </c>
+      <c r="D18">
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="E18">
+        <v>0.38095238095238093</v>
+      </c>
+      <c r="F18">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="G18">
+        <v>-0.46210205078125455</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>45560</v>
+      </c>
+      <c r="B19">
+        <v>87.131576538085938</v>
+      </c>
+      <c r="C19">
+        <v>89.35</v>
+      </c>
+      <c r="D19">
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="E19">
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="F19">
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="G19">
+        <v>-2.2184234619140568</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>45590</v>
+      </c>
+      <c r="B20">
+        <v>90.275001525878906</v>
+      </c>
+      <c r="C20">
+        <v>91.88</v>
+      </c>
+      <c r="D20">
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="E20">
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="F20">
+        <v>0.13636363636363635</v>
+      </c>
+      <c r="G20">
+        <v>-1.6049984741210892</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>45621</v>
+      </c>
+      <c r="B21">
+        <v>92.125</v>
+      </c>
+      <c r="C21">
+        <v>88.42</v>
+      </c>
+      <c r="D21">
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="E21">
+        <v>0.5</v>
+      </c>
+      <c r="F21">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="G21">
+        <v>3.7049999999999983</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>45651</v>
+      </c>
+      <c r="B22">
+        <v>91.526313781738281</v>
+      </c>
+      <c r="C22">
+        <v>83.16</v>
+      </c>
+      <c r="D22">
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="E22">
+        <v>0.5</v>
+      </c>
+      <c r="F22">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="G22">
+        <v>8.3663137817382847</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>45682</v>
+      </c>
+      <c r="B23">
+        <v>89.666664123535156</v>
+      </c>
+      <c r="C23">
+        <v>83.48</v>
+      </c>
+      <c r="D23">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E23">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="F23">
+        <v>9.5238095238095233E-2</v>
+      </c>
+      <c r="G23">
+        <v>6.1866641235351523</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>45713</v>
+      </c>
+      <c r="B24">
+        <v>89.3125</v>
+      </c>
+      <c r="C24">
+        <v>89.85</v>
+      </c>
+      <c r="D24">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E24">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="F24">
+        <v>9.5238095238095233E-2</v>
+      </c>
+      <c r="G24">
+        <v>-0.53749999999999432</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>45741</v>
+      </c>
+      <c r="B25">
+        <v>90.875</v>
+      </c>
+      <c r="C25">
+        <v>87.73</v>
+      </c>
+      <c r="D25">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E25">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="F25">
+        <v>9.5238095238095233E-2</v>
+      </c>
+      <c r="G25">
+        <v>3.144999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>45772</v>
+      </c>
+      <c r="B26">
+        <v>92.266670227050781</v>
+      </c>
+      <c r="C26">
+        <v>91.05</v>
+      </c>
+      <c r="D26">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E26">
+        <v>0.61904761904761907</v>
+      </c>
+      <c r="F26">
+        <v>4.7619047619047616E-2</v>
+      </c>
+      <c r="G26">
+        <v>1.2166702270507841</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -7809,25 +7466,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -8410,7 +8067,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -8425,25 +8082,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -9026,7 +8683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -9041,25 +8698,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -9642,7 +9299,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -9657,25 +9314,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -10258,7 +9915,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -10273,25 +9930,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -10874,7 +10531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -10889,25 +10546,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -11490,7 +11147,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -11505,25 +11162,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -12106,7 +11763,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -12121,25 +11778,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -12723,622 +12380,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G26"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>45041</v>
-      </c>
-      <c r="B2">
-        <v>72.1875</v>
-      </c>
-      <c r="C2">
-        <v>73.98</v>
-      </c>
-      <c r="D2">
-        <v>0.4</v>
-      </c>
-      <c r="E2">
-        <v>0.4</v>
-      </c>
-      <c r="F2">
-        <v>0.2</v>
-      </c>
-      <c r="G2">
-        <v>-1.792500000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>45071</v>
-      </c>
-      <c r="B3">
-        <v>72.875</v>
-      </c>
-      <c r="C3">
-        <v>69.819999999999993</v>
-      </c>
-      <c r="D3">
-        <v>0.42105263157894735</v>
-      </c>
-      <c r="E3">
-        <v>0.36842105263157893</v>
-      </c>
-      <c r="F3">
-        <v>0.21052631578947367</v>
-      </c>
-      <c r="G3">
-        <v>3.0550000000000068</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>45102</v>
-      </c>
-      <c r="B4">
-        <v>72.800003051757813</v>
-      </c>
-      <c r="C4">
-        <v>70.45</v>
-      </c>
-      <c r="D4">
-        <v>0.45</v>
-      </c>
-      <c r="E4">
-        <v>0.35</v>
-      </c>
-      <c r="F4">
-        <v>0.2</v>
-      </c>
-      <c r="G4">
-        <v>2.3500030517578097</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>45132</v>
-      </c>
-      <c r="B5">
-        <v>73.266670227050781</v>
-      </c>
-      <c r="C5">
-        <v>72.61</v>
-      </c>
-      <c r="D5">
-        <v>0.42105263157894735</v>
-      </c>
-      <c r="E5">
-        <v>0.31578947368421051</v>
-      </c>
-      <c r="F5">
-        <v>0.26315789473684209</v>
-      </c>
-      <c r="G5">
-        <v>0.65667022705078182</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>45163</v>
-      </c>
-      <c r="B6">
-        <v>72.894737243652344</v>
-      </c>
-      <c r="C6">
-        <v>68.09</v>
-      </c>
-      <c r="D6">
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="E6">
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="F6">
-        <v>9.5238095238095233E-2</v>
-      </c>
-      <c r="G6">
-        <v>4.8047372436523403</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>45194</v>
-      </c>
-      <c r="B7">
-        <v>73.052635192871094</v>
-      </c>
-      <c r="C7">
-        <v>69.290000000000006</v>
-      </c>
-      <c r="D7">
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="E7">
-        <v>0.52380952380952384</v>
-      </c>
-      <c r="F7">
-        <v>4.7619047619047616E-2</v>
-      </c>
-      <c r="G7">
-        <v>3.7626351928710875</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>45224</v>
-      </c>
-      <c r="B8">
-        <v>72.263160705566406</v>
-      </c>
-      <c r="C8">
-        <v>66.61</v>
-      </c>
-      <c r="D8">
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="E8">
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="F8">
-        <v>4.7619047619047616E-2</v>
-      </c>
-      <c r="G8">
-        <v>5.6531607055664068</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>45255</v>
-      </c>
-      <c r="B9">
-        <v>72.263160705566406</v>
-      </c>
-      <c r="C9">
-        <v>69.61</v>
-      </c>
-      <c r="D9">
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="E9">
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="F9">
-        <v>9.5238095238095233E-2</v>
-      </c>
-      <c r="G9">
-        <v>2.6531607055664068</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>45285</v>
-      </c>
-      <c r="B10">
-        <v>73.421051025390625</v>
-      </c>
-      <c r="C10">
-        <v>69.44</v>
-      </c>
-      <c r="D10">
-        <v>0.5</v>
-      </c>
-      <c r="E10">
-        <v>0.40909090909090912</v>
-      </c>
-      <c r="F10">
-        <v>9.0909090909090912E-2</v>
-      </c>
-      <c r="G10">
-        <v>3.9810510253906273</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>45316</v>
-      </c>
-      <c r="B11">
-        <v>74.599998474121094</v>
-      </c>
-      <c r="C11">
-        <v>69.239999999999995</v>
-      </c>
-      <c r="D11">
-        <v>0.54545454545454541</v>
-      </c>
-      <c r="E11">
-        <v>0.36363636363636365</v>
-      </c>
-      <c r="F11">
-        <v>9.0909090909090912E-2</v>
-      </c>
-      <c r="G11">
-        <v>5.3599984741210989</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>45347</v>
-      </c>
-      <c r="B12">
-        <v>73.421051025390625</v>
-      </c>
-      <c r="C12">
-        <v>67.69</v>
-      </c>
-      <c r="D12">
-        <v>0.54545454545454541</v>
-      </c>
-      <c r="E12">
-        <v>0.36363636363636365</v>
-      </c>
-      <c r="F12">
-        <v>9.0909090909090912E-2</v>
-      </c>
-      <c r="G12">
-        <v>5.7310510253906273</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>45376</v>
-      </c>
-      <c r="B13">
-        <v>73.368423461914063</v>
-      </c>
-      <c r="C13">
-        <v>69.760000000000005</v>
-      </c>
-      <c r="D13">
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="E13">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F13">
-        <v>9.5238095238095233E-2</v>
-      </c>
-      <c r="G13">
-        <v>3.6084234619140574</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>45407</v>
-      </c>
-      <c r="B14">
-        <v>73.611114501953125</v>
-      </c>
-      <c r="C14">
-        <v>74.37</v>
-      </c>
-      <c r="D14">
-        <v>0.52380952380952384</v>
-      </c>
-      <c r="E14">
-        <v>0.38095238095238093</v>
-      </c>
-      <c r="F14">
-        <v>9.5238095238095233E-2</v>
-      </c>
-      <c r="G14">
-        <v>-0.75888549804687955</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>45437</v>
-      </c>
-      <c r="B15">
-        <v>77.117645263671875</v>
-      </c>
-      <c r="C15">
-        <v>77.75</v>
-      </c>
-      <c r="D15">
-        <v>0.52380952380952384</v>
-      </c>
-      <c r="E15">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F15">
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="G15">
-        <v>-0.632354736328125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>45468</v>
-      </c>
-      <c r="B16">
-        <v>77.5</v>
-      </c>
-      <c r="C16">
-        <v>78.02</v>
-      </c>
-      <c r="D16">
-        <v>0.52380952380952384</v>
-      </c>
-      <c r="E16">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F16">
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="G16">
-        <v>-0.51999999999999602</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>45498</v>
-      </c>
-      <c r="B17">
-        <v>79.184211730957031</v>
-      </c>
-      <c r="C17">
-        <v>81.66</v>
-      </c>
-      <c r="D17">
-        <v>0.52380952380952384</v>
-      </c>
-      <c r="E17">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F17">
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="G17">
-        <v>-2.4757882690429653</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>45529</v>
-      </c>
-      <c r="B18">
-        <v>85.65789794921875</v>
-      </c>
-      <c r="C18">
-        <v>86.12</v>
-      </c>
-      <c r="D18">
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="E18">
-        <v>0.38095238095238093</v>
-      </c>
-      <c r="F18">
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="G18">
-        <v>-0.46210205078125455</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>45560</v>
-      </c>
-      <c r="B19">
-        <v>87.131576538085938</v>
-      </c>
-      <c r="C19">
-        <v>89.35</v>
-      </c>
-      <c r="D19">
-        <v>0.40909090909090912</v>
-      </c>
-      <c r="E19">
-        <v>0.45454545454545453</v>
-      </c>
-      <c r="F19">
-        <v>0.13636363636363635</v>
-      </c>
-      <c r="G19">
-        <v>-2.2184234619140568</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>45590</v>
-      </c>
-      <c r="B20">
-        <v>90.275001525878906</v>
-      </c>
-      <c r="C20">
-        <v>91.88</v>
-      </c>
-      <c r="D20">
-        <v>0.40909090909090912</v>
-      </c>
-      <c r="E20">
-        <v>0.45454545454545453</v>
-      </c>
-      <c r="F20">
-        <v>0.13636363636363635</v>
-      </c>
-      <c r="G20">
-        <v>-1.6049984741210892</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>45621</v>
-      </c>
-      <c r="B21">
-        <v>92.125</v>
-      </c>
-      <c r="C21">
-        <v>88.42</v>
-      </c>
-      <c r="D21">
-        <v>0.40909090909090912</v>
-      </c>
-      <c r="E21">
-        <v>0.5</v>
-      </c>
-      <c r="F21">
-        <v>9.0909090909090912E-2</v>
-      </c>
-      <c r="G21">
-        <v>3.7049999999999983</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>45651</v>
-      </c>
-      <c r="B22">
-        <v>91.526313781738281</v>
-      </c>
-      <c r="C22">
-        <v>83.16</v>
-      </c>
-      <c r="D22">
-        <v>0.40909090909090912</v>
-      </c>
-      <c r="E22">
-        <v>0.5</v>
-      </c>
-      <c r="F22">
-        <v>9.0909090909090912E-2</v>
-      </c>
-      <c r="G22">
-        <v>8.3663137817382847</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>45682</v>
-      </c>
-      <c r="B23">
-        <v>89.666664123535156</v>
-      </c>
-      <c r="C23">
-        <v>83.48</v>
-      </c>
-      <c r="D23">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E23">
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="F23">
-        <v>9.5238095238095233E-2</v>
-      </c>
-      <c r="G23">
-        <v>6.1866641235351523</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>45713</v>
-      </c>
-      <c r="B24">
-        <v>89.3125</v>
-      </c>
-      <c r="C24">
-        <v>89.85</v>
-      </c>
-      <c r="D24">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E24">
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="F24">
-        <v>9.5238095238095233E-2</v>
-      </c>
-      <c r="G24">
-        <v>-0.53749999999999432</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>45741</v>
-      </c>
-      <c r="B25">
-        <v>90.875</v>
-      </c>
-      <c r="C25">
-        <v>87.73</v>
-      </c>
-      <c r="D25">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E25">
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="F25">
-        <v>9.5238095238095233E-2</v>
-      </c>
-      <c r="G25">
-        <v>3.144999999999996</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>45772</v>
-      </c>
-      <c r="B26">
-        <v>92.266670227050781</v>
-      </c>
-      <c r="C26">
-        <v>91.05</v>
-      </c>
-      <c r="D26">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E26">
-        <v>0.61904761904761907</v>
-      </c>
-      <c r="F26">
-        <v>4.7619047619047616E-2</v>
-      </c>
-      <c r="G26">
-        <v>1.2166702270507841</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -13353,25 +12394,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -13954,7 +12995,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -13969,25 +13010,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -14570,7 +13611,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -14585,25 +13626,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -15186,7 +14227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -15201,25 +14242,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -15802,7 +14843,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -15817,25 +14858,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -16418,7 +15459,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -16433,25 +15474,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -17027,6 +16068,622 @@
       </c>
       <c r="G26">
         <v>72.326821899414057</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B2">
+        <v>159.5</v>
+      </c>
+      <c r="C2">
+        <v>152.36000000000001</v>
+      </c>
+      <c r="D2">
+        <v>0.48275862068965519</v>
+      </c>
+      <c r="E2">
+        <v>0.41379310344827586</v>
+      </c>
+      <c r="F2">
+        <v>0.10344827586206896</v>
+      </c>
+      <c r="G2">
+        <v>7.1399999999999864</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>45071</v>
+      </c>
+      <c r="B3">
+        <v>152.75</v>
+      </c>
+      <c r="C3">
+        <v>136.66</v>
+      </c>
+      <c r="D3">
+        <v>0.48275862068965519</v>
+      </c>
+      <c r="E3">
+        <v>0.41379310344827586</v>
+      </c>
+      <c r="F3">
+        <v>0.10344827586206896</v>
+      </c>
+      <c r="G3">
+        <v>16.090000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>45102</v>
+      </c>
+      <c r="B4">
+        <v>153</v>
+      </c>
+      <c r="C4">
+        <v>143.66999999999999</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+      <c r="E4">
+        <v>0.39285714285714285</v>
+      </c>
+      <c r="F4">
+        <v>0.10714285714285714</v>
+      </c>
+      <c r="G4">
+        <v>9.3300000000000125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45132</v>
+      </c>
+      <c r="B5">
+        <v>153.23809814453125</v>
+      </c>
+      <c r="C5">
+        <v>151.91999999999999</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+      <c r="E5">
+        <v>0.39285714285714285</v>
+      </c>
+      <c r="F5">
+        <v>0.10714285714285714</v>
+      </c>
+      <c r="G5">
+        <v>1.3180981445312625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45163</v>
+      </c>
+      <c r="B6">
+        <v>149.39131164550781</v>
+      </c>
+      <c r="C6">
+        <v>123.31</v>
+      </c>
+      <c r="D6">
+        <v>0.48275862068965519</v>
+      </c>
+      <c r="E6">
+        <v>0.41379310344827586</v>
+      </c>
+      <c r="F6">
+        <v>0.10344827586206896</v>
+      </c>
+      <c r="G6">
+        <v>26.08131164550781</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>45194</v>
+      </c>
+      <c r="B7">
+        <v>150.5238037109375</v>
+      </c>
+      <c r="C7">
+        <v>104.4</v>
+      </c>
+      <c r="D7">
+        <v>0.51724137931034486</v>
+      </c>
+      <c r="E7">
+        <v>0.37931034482758619</v>
+      </c>
+      <c r="F7">
+        <v>0.10344827586206896</v>
+      </c>
+      <c r="G7">
+        <v>46.123803710937494</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>45224</v>
+      </c>
+      <c r="B8">
+        <v>144.77272033691406</v>
+      </c>
+      <c r="C8">
+        <v>108.3</v>
+      </c>
+      <c r="D8">
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="E8">
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="F8">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="G8">
+        <v>36.472720336914065</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>45255</v>
+      </c>
+      <c r="B9">
+        <v>142.6842041015625</v>
+      </c>
+      <c r="C9">
+        <v>117.32</v>
+      </c>
+      <c r="D9">
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="E9">
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="F9">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="G9">
+        <v>25.364204101562507</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>45285</v>
+      </c>
+      <c r="B10">
+        <v>143.52174377441406</v>
+      </c>
+      <c r="C10">
+        <v>136.56</v>
+      </c>
+      <c r="D10">
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="E10">
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="F10">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="G10">
+        <v>6.9617437744140602</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>45316</v>
+      </c>
+      <c r="B11">
+        <v>145.2608642578125</v>
+      </c>
+      <c r="C11">
+        <v>132.22999999999999</v>
+      </c>
+      <c r="D11">
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="E11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F11">
+        <v>0.1</v>
+      </c>
+      <c r="G11">
+        <v>13.03086425781251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>45347</v>
+      </c>
+      <c r="B12">
+        <v>148</v>
+      </c>
+      <c r="C12">
+        <v>145.88</v>
+      </c>
+      <c r="D12">
+        <v>0.6</v>
+      </c>
+      <c r="E12">
+        <v>0.3</v>
+      </c>
+      <c r="F12">
+        <v>0.1</v>
+      </c>
+      <c r="G12">
+        <v>2.1200000000000045</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>45376</v>
+      </c>
+      <c r="B13">
+        <v>148.69564819335938</v>
+      </c>
+      <c r="C13">
+        <v>126.15</v>
+      </c>
+      <c r="D13">
+        <v>0.58620689655172409</v>
+      </c>
+      <c r="E13">
+        <v>0.34482758620689657</v>
+      </c>
+      <c r="F13">
+        <v>6.8965517241379309E-2</v>
+      </c>
+      <c r="G13">
+        <v>22.545648193359369</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>45407</v>
+      </c>
+      <c r="B14">
+        <v>148.65217590332031</v>
+      </c>
+      <c r="C14">
+        <v>121.69</v>
+      </c>
+      <c r="D14">
+        <v>0.55172413793103448</v>
+      </c>
+      <c r="E14">
+        <v>0.37931034482758619</v>
+      </c>
+      <c r="F14">
+        <v>6.8965517241379309E-2</v>
+      </c>
+      <c r="G14">
+        <v>26.962175903320315</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>45437</v>
+      </c>
+      <c r="B15">
+        <v>147.75</v>
+      </c>
+      <c r="C15">
+        <v>115.37</v>
+      </c>
+      <c r="D15">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="E15">
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="F15">
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="G15">
+        <v>32.379999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>45468</v>
+      </c>
+      <c r="B16">
+        <v>137.29167175292969</v>
+      </c>
+      <c r="C16">
+        <v>105.41</v>
+      </c>
+      <c r="D16">
+        <v>0.5357142857142857</v>
+      </c>
+      <c r="E16">
+        <v>0.39285714285714285</v>
+      </c>
+      <c r="F16">
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="G16">
+        <v>31.881671752929691</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>45498</v>
+      </c>
+      <c r="B17">
+        <v>136.36000061035156</v>
+      </c>
+      <c r="C17">
+        <v>102.63</v>
+      </c>
+      <c r="D17">
+        <v>0.5</v>
+      </c>
+      <c r="E17">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="F17">
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="G17">
+        <v>33.730000610351567</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>45529</v>
+      </c>
+      <c r="B18">
+        <v>133</v>
+      </c>
+      <c r="C18">
+        <v>97</v>
+      </c>
+      <c r="D18">
+        <v>0.5357142857142857</v>
+      </c>
+      <c r="E18">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="F18">
+        <v>3.5714285714285712E-2</v>
+      </c>
+      <c r="G18">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>45560</v>
+      </c>
+      <c r="B19">
+        <v>82.615386962890625</v>
+      </c>
+      <c r="C19">
+        <v>70.55</v>
+      </c>
+      <c r="D19">
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="E19">
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="F19">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="G19">
+        <v>12.065386962890628</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>45590</v>
+      </c>
+      <c r="B20">
+        <v>83.296295166015625</v>
+      </c>
+      <c r="C20">
+        <v>66.45</v>
+      </c>
+      <c r="D20">
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="E20">
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="F20">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="G20">
+        <v>16.846295166015622</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>45621</v>
+      </c>
+      <c r="B21">
+        <v>81.615386962890625</v>
+      </c>
+      <c r="C21">
+        <v>69.78</v>
+      </c>
+      <c r="D21">
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="E21">
+        <v>0.6</v>
+      </c>
+      <c r="F21">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="G21">
+        <v>11.835386962890624</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>45651</v>
+      </c>
+      <c r="B22">
+        <v>83.538459777832031</v>
+      </c>
+      <c r="C22">
+        <v>73.38</v>
+      </c>
+      <c r="D22">
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="E22">
+        <v>0.6</v>
+      </c>
+      <c r="F22">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="G22">
+        <v>10.158459777832036</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>45682</v>
+      </c>
+      <c r="B23">
+        <v>84.038459777832031</v>
+      </c>
+      <c r="C23">
+        <v>72.48</v>
+      </c>
+      <c r="D23">
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="E23">
+        <v>0.6</v>
+      </c>
+      <c r="F23">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="G23">
+        <v>11.558459777832027</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>45713</v>
+      </c>
+      <c r="B24">
+        <v>83.653846740722656</v>
+      </c>
+      <c r="C24">
+        <v>76.22</v>
+      </c>
+      <c r="D24">
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="E24">
+        <v>0.6</v>
+      </c>
+      <c r="F24">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="G24">
+        <v>7.4338467407226574</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>45741</v>
+      </c>
+      <c r="B25">
+        <v>79.941177368164063</v>
+      </c>
+      <c r="C25">
+        <v>67.14</v>
+      </c>
+      <c r="D25">
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="E25">
+        <v>0.6</v>
+      </c>
+      <c r="F25">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="G25">
+        <v>12.801177368164062</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>45772</v>
+      </c>
+      <c r="B26">
+        <v>82.954544067382813</v>
+      </c>
+      <c r="C26">
+        <v>81.23</v>
+      </c>
+      <c r="D26">
+        <v>0.41379310344827586</v>
+      </c>
+      <c r="E26">
+        <v>0.55172413793103448</v>
+      </c>
+      <c r="F26">
+        <v>3.4482758620689655E-2</v>
+      </c>
+      <c r="G26">
+        <v>1.7245440673828085</v>
       </c>
     </row>
   </sheetData>

</xml_diff>